<commit_message>
updated template and template_type to remove duplicate template type code.
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10A25E7-F483-4FEC-9FF5-FDD52262045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FCA463-3D86-4AC6-9C36-CA205CF91E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7048" uniqueCount="686">
   <si>
     <t>lang_code</t>
   </si>
@@ -2080,13 +2080,19 @@
   </si>
   <si>
     <t>Locked status</t>
+  </si>
+  <si>
+    <t>reg-consent-template</t>
+  </si>
+  <si>
+    <t>Registration Client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2117,6 +2123,12 @@
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2154,7 +2166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2170,6 +2182,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2478,10 +2491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1761"/>
+  <dimension ref="A1:D1762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1743" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1750" sqref="B1750"/>
+    <sheetView tabSelected="1" topLeftCell="A1758" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1763" sqref="C1763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -27145,6 +27158,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1762" spans="1:4">
+      <c r="A1762" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1762" t="s">
+        <v>684</v>
+      </c>
+      <c r="C1762" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="D1762" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1761" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>